<commit_message>
Added data saving and prepare for quant
</commit_message>
<xml_diff>
--- a/LayerOutputCalculator.xlsx
+++ b/LayerOutputCalculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/251453d765650dfd/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/251453d765650dfd/Documents/SCNNResearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{A13430F1-7776-49D8-9039-3A2D28A9D9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C27FCCB3-2AFA-4409-AEC6-833C121BB01F}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="8_{A13430F1-7776-49D8-9039-3A2D28A9D9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09476460-3A37-4167-A739-23655CD51905}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{016CB15B-A114-44E4-9337-D080E4979728}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{016CB15B-A114-44E4-9337-D080E4979728}"/>
   </bookViews>
   <sheets>
     <sheet name="Conv" sheetId="1" r:id="rId1"/>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03CF7DCE-D1F7-44D4-A7A7-83F8CB9B73B8}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,13 +956,13 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
       </c>
       <c r="E1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -970,13 +970,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1001,12 +1001,13 @@
       </c>
       <c r="B6">
         <f>($B$1-$B$2+(2*$B$3))/$B$4 + 1</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6">
+        <f>E2</f>
         <v>8</v>
       </c>
     </row>
@@ -1021,7 +1022,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1122,7 +1123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03446D2B-F60A-4083-87E6-05A051C137EE}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>